<commit_message>
Complete merging develop into StorageBOSSE
</commit_message>
<xml_diff>
--- a/labor_cost_sensitivity_outputs.xlsx
+++ b/labor_cost_sensitivity_outputs.xlsx
@@ -344,7 +344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1444,6 +1444,146 @@
         <v>50.2336140771021</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>area undefined</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>100</v>
+      </c>
+      <c r="D16" t="n">
+        <v>100</v>
+      </c>
+      <c r="E16" t="n">
+        <v>124517501.1612876</v>
+      </c>
+      <c r="F16" t="n">
+        <v>100000000</v>
+      </c>
+      <c r="G16" t="n">
+        <v>24517501.16128756</v>
+      </c>
+      <c r="H16" t="n">
+        <v>16332027.26010531</v>
+      </c>
+      <c r="I16" t="n">
+        <v>116302.8620469598</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2956469.651481002</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1049740.5</v>
+      </c>
+      <c r="L16" t="n">
+        <v>11539361.24657734</v>
+      </c>
+      <c r="M16" t="n">
+        <v>615203</v>
+      </c>
+      <c r="N16" t="n">
+        <v>54950</v>
+      </c>
+      <c r="O16" t="n">
+        <v>8185473.901182257</v>
+      </c>
+      <c r="P16" t="n">
+        <v>19.69000416216997</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>12191684.05266326</v>
+      </c>
+      <c r="R16" t="n">
+        <v>49.72645447209597</v>
+      </c>
+      <c r="S16" t="n">
+        <v>12307986.91471022</v>
+      </c>
+      <c r="T16" t="n">
+        <v>50.20082117562691</v>
+      </c>
+      <c r="U16" t="n">
+        <v>12316026.91471022</v>
+      </c>
+      <c r="V16" t="n">
+        <v>50.2336140771021</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>area undefined</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" t="n">
+        <v>100</v>
+      </c>
+      <c r="E17" t="n">
+        <v>124517501.1612876</v>
+      </c>
+      <c r="F17" t="n">
+        <v>100000000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>24517501.16128756</v>
+      </c>
+      <c r="H17" t="n">
+        <v>16332027.26010531</v>
+      </c>
+      <c r="I17" t="n">
+        <v>116302.8620469598</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2956469.651481002</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1049740.5</v>
+      </c>
+      <c r="L17" t="n">
+        <v>11539361.24657734</v>
+      </c>
+      <c r="M17" t="n">
+        <v>615203</v>
+      </c>
+      <c r="N17" t="n">
+        <v>54950</v>
+      </c>
+      <c r="O17" t="n">
+        <v>8185473.901182257</v>
+      </c>
+      <c r="P17" t="n">
+        <v>19.69000416216997</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>12191684.05266326</v>
+      </c>
+      <c r="R17" t="n">
+        <v>49.72645447209597</v>
+      </c>
+      <c r="S17" t="n">
+        <v>12307986.91471022</v>
+      </c>
+      <c r="T17" t="n">
+        <v>50.20082117562691</v>
+      </c>
+      <c r="U17" t="n">
+        <v>12316026.91471022</v>
+      </c>
+      <c r="V17" t="n">
+        <v>50.2336140771021</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>